<commit_message>
Repository Backlog [Kat - 21 March]
</commit_message>
<xml_diff>
--- a/burndownChart.xlsx
+++ b/burndownChart.xlsx
@@ -1243,16 +1243,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2700</c:v>
+                  <c:v>2350</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2179,7 +2179,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2245,8 +2245,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="18">
-        <f>900*3</f>
-        <v>2700</v>
+        <v>2350</v>
       </c>
       <c r="C6" s="19">
         <v>0</v>
@@ -2264,7 +2263,7 @@
       </c>
       <c r="G6" s="17">
         <f>B6-D6</f>
-        <v>2700</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -2272,7 +2271,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="18">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C7" s="19">
         <v>0</v>
@@ -2290,7 +2289,7 @@
       </c>
       <c r="G7" s="17">
         <f>B7-D7</f>
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -2298,7 +2297,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="18">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C8" s="18">
         <v>0</v>
@@ -2317,7 +2316,7 @@
       </c>
       <c r="G8" s="17">
         <f>B8-D8</f>
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2325,7 +2324,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="18">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C9" s="18">
         <v>0</v>
@@ -2344,7 +2343,7 @@
       </c>
       <c r="G9" s="17">
         <f>B9-D9</f>
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -2493,7 +2492,13 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><_dlc_DocId xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07">WORK-769-155</_dlc_DocId><_dlc_DocIdUrl xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07"><Url>http://intranet/workingtogether/projects/110405/_layouts/DocIdRedir.aspx?ID=WORK-769-155</Url><Description>WORK-769-155</Description></_dlc_DocIdUrl><IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/><Last_x0020_Archive xmlns="$ListId:Shared Documents;" xsi:nil="true"/><Reason xmlns="$ListId:Shared Documents;" xsi:nil="true"></Reason></documentManagement></p:properties>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2542,13 +2547,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><_dlc_DocId xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07">WORK-769-155</_dlc_DocId><_dlc_DocIdUrl xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07"><Url>http://intranet/workingtogether/projects/110405/_layouts/DocIdRedir.aspx?ID=WORK-769-155</Url><Description>WORK-769-155</Description></_dlc_DocIdUrl><IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/><Last_x0020_Archive xmlns="$ListId:Shared Documents;" xsi:nil="true"/><Reason xmlns="$ListId:Shared Documents;" xsi:nil="true"></Reason></documentManagement></p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F770ABC8F9B27C4C8461F4575C23FAEA" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6f0f4afd6cc55b40f57cb0d59e49aa45" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
@@ -2726,6 +2725,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8575168F-6331-41DA-B879-8152475B9854}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29BDFB93-A148-4832-8767-0A894C12A9C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C0C9F9C-98B5-480F-B2D6-CAE7CFAF0133}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -2739,22 +2754,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
     <ds:schemaRef ds:uri="0d93dc7d-5998-434b-bf34-aa89b432ec07"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29BDFB93-A148-4832-8767-0A894C12A9C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8575168F-6331-41DA-B879-8152475B9854}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>